<commit_message>
Feedback and Security tests fixed
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="R1 Regression" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -49,40 +49,46 @@
     <t>Card Id</t>
   </si>
   <si>
+    <t>Pa$$w0rd</t>
+  </si>
+  <si>
+    <t>Wipro1234</t>
+  </si>
+  <si>
+    <t>SNSWSN</t>
+  </si>
+  <si>
+    <t>TC Name</t>
+  </si>
+  <si>
+    <t>test1623@mailinator.com</t>
+  </si>
+  <si>
+    <t>Snsw123#</t>
+  </si>
+  <si>
+    <t>SNSWFeedBackTest</t>
+  </si>
+  <si>
+    <t>SNSWUpdateSecurityQTest</t>
+  </si>
+  <si>
+    <t>SNSWLinkingTestA</t>
+  </si>
+  <si>
     <t>sa021@mailinator.com</t>
   </si>
   <si>
-    <t>Pa$$w0rd</t>
-  </si>
-  <si>
-    <t>Wipro1234</t>
-  </si>
-  <si>
-    <t>sa020@mailinator.com</t>
-  </si>
-  <si>
-    <t>sa015@mailinator.com</t>
-  </si>
-  <si>
-    <t>SNSWSN</t>
-  </si>
-  <si>
-    <t>ADSSN</t>
-  </si>
-  <si>
-    <t>ADSFN</t>
-  </si>
-  <si>
-    <t>PARRAMATTA</t>
-  </si>
-  <si>
-    <t>TC Name</t>
+    <t>SNSWLinkingTestB</t>
+  </si>
+  <si>
+    <t>SNSWLinkingTestC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,10 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -215,6 +222,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -250,6 +274,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,16 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
@@ -450,7 +491,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -487,60 +528,74 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>45166444</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>45164772</v>
-      </c>
-      <c r="G3">
-        <v>98951843</v>
-      </c>
-      <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>45164772</v>
+      </c>
+      <c r="G4">
+        <v>98951843</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>45166444</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F4">
-        <v>45167406</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="2">
-        <v>17085</v>
-      </c>
-      <c r="K4">
-        <v>2140</v>
-      </c>
-      <c r="L4" t="s">
-        <v>19</v>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check Demerits test added
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>SNSWLinkingTestC</t>
+  </si>
+  <si>
+    <t>CheckDemeritsTest</t>
+  </si>
+  <si>
+    <t>sa020@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -467,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +604,17 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Data - Option B Linking Details Added
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>sa020@mailinator.com</t>
+  </si>
+  <si>
+    <t>7 KEVIN RD, ALBION PARK NSW 2527</t>
+  </si>
+  <si>
+    <t>Mailing Address</t>
+  </si>
+  <si>
+    <t>Residential Adress</t>
   </si>
 </sst>
 </file>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K10" sqref="K10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,9 +502,10 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -532,8 +542,14 @@
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -544,7 +560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -555,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -575,8 +591,14 @@
         <v>13</v>
       </c>
       <c r="J4" s="2"/>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -593,7 +615,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -604,7 +626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
linking option c test
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>Residential Adress</t>
+  </si>
+  <si>
+    <t>ADSSN</t>
+  </si>
+  <si>
+    <t>ADSFN</t>
+  </si>
+  <si>
+    <t>PARRAMATTA</t>
+  </si>
+  <si>
+    <t>10/10/1975</t>
   </si>
 </sst>
 </file>
@@ -139,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +498,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10:K11"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,8 +513,8 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
     <col min="13" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -537,10 +550,10 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>27</v>
@@ -624,6 +637,24 @@
       </c>
       <c r="C6" t="s">
         <v>11</v>
+      </c>
+      <c r="D6">
+        <v>45171943</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6">
+        <v>2140</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Linking option C test fixed
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>10/10/1975</t>
+  </si>
+  <si>
+    <t>sa019@mailinator.com</t>
+  </si>
+  <si>
+    <t>UNIT 35, 146-152 PARRAMATTA RD, HOMEBUSH NSW 2140</t>
   </si>
 </sst>
 </file>
@@ -497,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +639,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -655,6 +661,12 @@
       </c>
       <c r="L6">
         <v>2140</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -670,5 +682,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DS - Option A RMS Linking Test
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>sa020@mailinator.com</t>
-  </si>
-  <si>
-    <t>7 KEVIN RD, ALBION PARK NSW 2527</t>
   </si>
   <si>
     <t>Mailing Address</t>
@@ -503,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,10 +559,10 @@
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -611,10 +608,10 @@
       </c>
       <c r="J4" s="2"/>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -633,13 +630,19 @@
       <c r="E5" t="s">
         <v>12</v>
       </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -648,25 +651,25 @@
         <v>45171943</v>
       </c>
       <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" t="s">
         <v>29</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
       </c>
       <c r="L6">
         <v>2140</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DS - Address Change - Login, Guest , Email and Mobile Changes
</commit_message>
<xml_diff>
--- a/test/r1regression/testdata.xlsx
+++ b/test/r1regression/testdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="5955"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Username</t>
   </si>
@@ -88,9 +88,6 @@
     <t>CheckDemeritsTest</t>
   </si>
   <si>
-    <t>sa020@mailinator.com</t>
-  </si>
-  <si>
     <t>Mailing Address</t>
   </si>
   <si>
@@ -112,7 +109,31 @@
     <t>sa019@mailinator.com</t>
   </si>
   <si>
+    <t>ChangeAddressDetailsTest</t>
+  </si>
+  <si>
+    <t>ChangeAddressDetailsGuestTest</t>
+  </si>
+  <si>
+    <t>ChangeMobileAndEmailTest</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
     <t>UNIT 35, 146-152 PARRAMATTA RD, HOMEBUSH NSW 2140</t>
+  </si>
+  <si>
+    <t>UNIT 66, 653-659 GEORGE ST, HAYMARKET NSW 2000</t>
+  </si>
+  <si>
+    <t>sa021@mailinator4.com</t>
+  </si>
+  <si>
+    <t>0451764467</t>
   </si>
 </sst>
 </file>
@@ -154,12 +175,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,15 +521,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
@@ -518,10 +541,12 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -559,13 +584,19 @@
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -576,7 +607,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -587,7 +618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -608,13 +639,13 @@
       </c>
       <c r="J4" s="2"/>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -631,18 +662,18 @@
         <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -651,36 +682,79 @@
         <v>45171943</v>
       </c>
       <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
         <v>27</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
         <v>28</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>29</v>
       </c>
       <c r="L6">
         <v>2140</v>
       </c>
       <c r="M6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="F9">
+        <v>45164185</v>
+      </c>
+      <c r="G9">
+        <v>98951626</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>